<commit_message>
Updated the documentation, weight and cost
</commit_message>
<xml_diff>
--- a/documents/Documentation.xlsx
+++ b/documents/Documentation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Centralizare" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,9 +19,9 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">Carcasă!$A$3:$F$195</definedName>
-    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">Circuit!$A$3:$F$200</definedName>
+    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">Circuit!$A$3:$F$201</definedName>
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Pini!$A$3:$D$194</definedName>
-    <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">Structură!$A$3:$F$210</definedName>
+    <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">Structură!$A$3:$F$209</definedName>
     <definedName function="false" hidden="true" localSheetId="7" name="_xlnm._FilterDatabase" vbProcedure="false">Telecomandă!$A$3:$F$181</definedName>
     <definedName function="false" hidden="false" name="capacityList" vbProcedure="false">Alimentare!$T:$T</definedName>
     <definedName function="false" hidden="false" name="voltageList" vbProcedure="false">Alimentare!$R:$R</definedName>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="120">
   <si>
     <t xml:space="preserve">Componentă</t>
   </si>
@@ -119,7 +119,7 @@
     <t xml:space="preserve">Compartiment 1 – Elice</t>
   </si>
   <si>
-    <t xml:space="preserve">Compartiment 2</t>
+    <t xml:space="preserve">Compartiment 2 – Provă</t>
   </si>
   <si>
     <t xml:space="preserve">Compartiment 3</t>
@@ -137,10 +137,10 @@
     <t xml:space="preserve">Compartiment 7</t>
   </si>
   <si>
-    <t xml:space="preserve">Compartiment 8</t>
+    <t xml:space="preserve">Compartiment 8 – Pupă</t>
   </si>
   <si>
-    <t xml:space="preserve">Compartiment 9</t>
+    <t xml:space="preserve">Compartiment 9 – Corpul de navigație</t>
   </si>
   <si>
     <t xml:space="preserve">Cârmă</t>
@@ -242,35 +242,7 @@
     <t xml:space="preserve">Senzor inerțial MPU9250</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF333333"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Senzor m</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF333333"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">icromotor</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF333333"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> HPCB 6 V cu ax lung</t>
-    </r>
+    <t xml:space="preserve">Senzor micromotor HPCB 6 V cu ax lung</t>
   </si>
   <si>
     <t xml:space="preserve">Servomotor MG996R 60</t>
@@ -298,6 +270,9 @@
   </si>
   <si>
     <t xml:space="preserve">Acumulator 1.6V 1500 mAh AA Ansmann</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mini Breadboard negru</t>
   </si>
   <si>
     <t xml:space="preserve">Placă de dezvoltare Arduino Nano V3</t>
@@ -348,58 +323,40 @@
     <t xml:space="preserve">Structură</t>
   </si>
   <si>
-    <t xml:space="preserve">Bandă asamblare oțel zincat 200 mm</t>
+    <t xml:space="preserve">Bandă asamblare oțel zincat  60 mm</t>
   </si>
   <si>
-    <t xml:space="preserve">Bandă asamblare oțel zincat 60 mm</t>
+    <t xml:space="preserve">Bandă asamblare oțel zincat  80 mm</t>
   </si>
   <si>
-    <t xml:space="preserve">Bandă asamblare oțel zincat 80 mm</t>
+    <t xml:space="preserve">Bandă asamblare oțel zincat 200 mm</t>
   </si>
   <si>
     <t xml:space="preserve">Capac borcan metalic auriu 90 mm</t>
   </si>
   <si>
-    <t xml:space="preserve">Colțar Cutii Zinc 36x36x36 mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Colțar Cutii Zinc 50x50x50 mm</t>
-  </si>
-  <si>
     <t xml:space="preserve">Conector L dreapta Zinc 30x40x1 mm</t>
   </si>
   <si>
-    <t xml:space="preserve">Conector unghi Zinc 30x30x1 mm</t>
+    <t xml:space="preserve">Conector unghi Zinc 30x30x15 mm</t>
   </si>
   <si>
     <t xml:space="preserve">Cornier Negru cu Șuruburi pentru Motoarele N20 </t>
   </si>
   <si>
+    <t xml:space="preserve">Bară cilindrică hot glue 11x300 mm</t>
+  </si>
+  <si>
     <t xml:space="preserve">Magnet adeziv disc 12 mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PET 1.5 l</t>
   </si>
   <si>
     <t xml:space="preserve">Pilon M3 18 mm</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF333333"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Pilon M3 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF333333"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">25 mm</t>
-    </r>
+    <t xml:space="preserve">Pilon M3 25 mm</t>
   </si>
   <si>
     <t xml:space="preserve">Piuliță M3 hexagonală</t>
@@ -411,70 +368,19 @@
     <t xml:space="preserve">Șaibă M3</t>
   </si>
   <si>
+    <t xml:space="preserve">Șuruburi M3  4 mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Șuruburi M3  8 mm</t>
+  </si>
+  <si>
     <t xml:space="preserve">Șuruburi M3 16 mm</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF333333"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Șuruburi M3 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF333333"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">25 mm</t>
-    </r>
+    <t xml:space="preserve">Șuruburi M3 25 mm</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF333333"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Șuruburi M3 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF333333"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">45 mm</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF333333"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Șuruburi M3 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF333333"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">8 mm</t>
-    </r>
+    <t xml:space="preserve">Șuruburi M3 45 mm</t>
   </si>
   <si>
     <t xml:space="preserve">Tijă filetată M3 1 m</t>
@@ -483,7 +389,7 @@
     <t xml:space="preserve">Carcasă</t>
   </si>
   <si>
-    <t xml:space="preserve">Silicon</t>
+    <t xml:space="preserve">Silicon 300ml</t>
   </si>
   <si>
     <t xml:space="preserve">PET 1.5 L</t>
@@ -618,12 +524,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FFEEEEEC"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -635,6 +535,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1301,7 +1207,7 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1321,11 +1227,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="181" fontId="17" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="181" fontId="16" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1345,7 +1251,7 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="15" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="17" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1514,7 +1420,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="18.38"/>
@@ -1585,11 +1491,11 @@
       </c>
       <c r="B2" s="17" t="n">
         <f aca="true">INDIRECT(ADDRESS(Centralizare!$D$2, Centralizare!$D$3, 1, 1, Centralizare!$A2), 1)</f>
-        <v>1364.9</v>
+        <v>1374.34</v>
       </c>
       <c r="C2" s="18" t="n">
         <f aca="true">INDIRECT(ADDRESS(Centralizare!$D$2, Centralizare!$D$4, 1, 1, Centralizare!$A2), 1)</f>
-        <v>1708.59</v>
+        <v>1764.59</v>
       </c>
       <c r="D2" s="14" t="n">
         <v>2</v>
@@ -1620,7 +1526,7 @@
       </c>
       <c r="M2" s="25" t="n">
         <f aca="false">C5 / 1000</f>
-        <v>7.17934</v>
+        <v>6.209994</v>
       </c>
       <c r="N2" s="25" t="n">
         <f aca="false">J2 * K2</f>
@@ -1628,7 +1534,7 @@
       </c>
       <c r="O2" s="26" t="n">
         <f aca="false">L2 * M2 / N2</f>
-        <v>0.0913909171419811</v>
+        <v>0.0790514235439748</v>
       </c>
       <c r="AMB2" s="0"/>
       <c r="AMC2" s="0"/>
@@ -1647,11 +1553,11 @@
       </c>
       <c r="B3" s="28" t="n">
         <f aca="true">INDIRECT(ADDRESS(Centralizare!$D$2, Centralizare!$D$3, 1, 1, Centralizare!$A3), 1)</f>
-        <v>442.938</v>
+        <v>453.38</v>
       </c>
       <c r="C3" s="29" t="n">
         <f aca="true">INDIRECT(ADDRESS(Centralizare!$D$2, Centralizare!$D$4, 1, 1, Centralizare!$A3), 1)</f>
-        <v>4170.75</v>
+        <v>3080.404</v>
       </c>
       <c r="D3" s="14" t="n">
         <v>4</v>
@@ -1687,11 +1593,11 @@
       </c>
       <c r="B4" s="31" t="n">
         <f aca="true">INDIRECT(ADDRESS(Centralizare!$D$2, Centralizare!$D$3, 1, 1, Centralizare!$A4), 1)</f>
-        <v>94</v>
+        <v>190</v>
       </c>
       <c r="C4" s="32" t="n">
         <f aca="true">INDIRECT(ADDRESS(Centralizare!$D$2, Centralizare!$D$4, 1, 1, Centralizare!$A4), 1)</f>
-        <v>1300</v>
+        <v>1365</v>
       </c>
       <c r="D4" s="14" t="n">
         <v>6</v>
@@ -1725,12 +1631,12 @@
         <v>16</v>
       </c>
       <c r="B5" s="34" t="n">
-        <f aca="false">IF(SUM(B1:B3), SUM(B1:B3), "")</f>
-        <v>1807.838</v>
+        <f aca="false">IF(SUM(B2:B4), SUM(B2:B4), "")</f>
+        <v>2017.72</v>
       </c>
       <c r="C5" s="35" t="n">
         <f aca="false">IF(SUM(C2:C3), SUM(C2:C4), "")</f>
-        <v>7179.34</v>
+        <v>6209.994</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="19" t="n">
@@ -1777,11 +1683,11 @@
       </c>
       <c r="B7" s="40" t="n">
         <f aca="false">IF(SUM(B5:B6), SUM(B5:B6), "")</f>
-        <v>1863.838</v>
+        <v>2073.72</v>
       </c>
       <c r="C7" s="41" t="n">
         <f aca="false">IF(SUM(C5:C6), SUM(C5:C6), "")</f>
-        <v>7304.34</v>
+        <v>6334.994</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1807,11 +1713,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="15.56"/>
@@ -1951,6 +1857,7 @@
         <v>0.13</v>
       </c>
       <c r="C4" s="26" t="n">
+        <f aca="false">C3</f>
         <v>0.1</v>
       </c>
       <c r="D4" s="43" t="n">
@@ -1993,6 +1900,7 @@
         <v>0.13</v>
       </c>
       <c r="C5" s="26" t="n">
+        <f aca="false">C3</f>
         <v>0.1</v>
       </c>
       <c r="D5" s="43" t="n">
@@ -2035,6 +1943,7 @@
         <v>0.25</v>
       </c>
       <c r="C6" s="26" t="n">
+        <f aca="false">C3</f>
         <v>0.1</v>
       </c>
       <c r="D6" s="43" t="n">
@@ -2050,11 +1959,11 @@
         <v>0.025</v>
       </c>
       <c r="G6" s="44" t="n">
-        <v>160</v>
+        <v>250</v>
       </c>
       <c r="H6" s="45" t="n">
         <f aca="false">G6/Centralizare!$K$2/F6</f>
-        <v>6.4</v>
+        <v>10</v>
       </c>
       <c r="ALY6" s="0"/>
       <c r="ALZ6" s="0"/>
@@ -2077,6 +1986,7 @@
         <v>0.13</v>
       </c>
       <c r="C7" s="26" t="n">
+        <f aca="false">C3</f>
         <v>0.1</v>
       </c>
       <c r="D7" s="43" t="n">
@@ -2119,6 +2029,7 @@
         <v>0.13</v>
       </c>
       <c r="C8" s="26" t="n">
+        <f aca="false">C3</f>
         <v>0.1</v>
       </c>
       <c r="D8" s="43" t="n">
@@ -2161,6 +2072,7 @@
         <v>0.085</v>
       </c>
       <c r="C9" s="26" t="n">
+        <f aca="false">C3</f>
         <v>0.1</v>
       </c>
       <c r="D9" s="43" t="n">
@@ -2176,11 +2088,11 @@
         <v>0.0085</v>
       </c>
       <c r="G9" s="44" t="n">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H9" s="45" t="n">
         <f aca="false">G9/Centralizare!$K$2/F9</f>
-        <v>9.41176470588235</v>
+        <v>10</v>
       </c>
       <c r="ALY9" s="0"/>
       <c r="ALZ9" s="0"/>
@@ -2382,7 +2294,7 @@
       <c r="G14" s="44"/>
       <c r="H14" s="45" t="n">
         <f aca="false">MIN(H2:H13)</f>
-        <v>6.4</v>
+        <v>10</v>
       </c>
       <c r="ALY14" s="0"/>
       <c r="ALZ14" s="0"/>
@@ -2421,7 +2333,7 @@
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="19.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="19.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="46" width="25.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="47" width="10.19"/>
@@ -3280,7 +3192,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="84" width="50.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="85" width="21.95"/>
@@ -3632,10 +3544,10 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="19.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="19.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="84" width="55.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="86" width="16.81"/>
@@ -3681,23 +3593,23 @@
       </c>
       <c r="B2" s="97" t="n">
         <f aca="true">IF(SUM(INDIRECT(B1)), SUM(INDIRECT(B1)), "")</f>
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C2" s="17" t="n">
         <f aca="true">IF(SUM(INDIRECT(C1)), AVERAGE(INDIRECT(C1)), "")</f>
-        <v>18.925</v>
+        <v>18.1361904761905</v>
       </c>
       <c r="D2" s="17" t="n">
         <f aca="true">IF(SUM(INDIRECT(D1)), SUM(INDIRECT(D1)), "")</f>
-        <v>1364.9</v>
+        <v>1374.34</v>
       </c>
       <c r="E2" s="102" t="n">
         <f aca="true">IF(SUM(INDIRECT(E1)), AVERAGE(INDIRECT(E1)), "")</f>
-        <v>15.0675</v>
+        <v>15.0166666666667</v>
       </c>
       <c r="F2" s="102" t="n">
         <f aca="true">IF(SUM(INDIRECT(F1)), SUM(INDIRECT(F1)), "")</f>
-        <v>1708.59</v>
+        <v>1764.59</v>
       </c>
       <c r="G2" s="103"/>
     </row>
@@ -3769,22 +3681,22 @@
       <c r="A6" s="84" t="s">
         <v>78</v>
       </c>
-      <c r="B6" s="86" t="n">
-        <v>2</v>
+      <c r="B6" s="106" t="n">
+        <v>4</v>
       </c>
       <c r="C6" s="88" t="n">
-        <v>20</v>
+        <v>2.36</v>
       </c>
       <c r="D6" s="88" t="n">
         <f aca="false">IF(Circuit!B6, Circuit!B6 * Circuit!C6, "")</f>
-        <v>40</v>
+        <v>9.44</v>
       </c>
       <c r="E6" s="101" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F6" s="101" t="n">
         <f aca="false">IF(Circuit!B6, Circuit!B6 * Circuit!E6, "")</f>
-        <v>34</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3792,21 +3704,21 @@
         <v>79</v>
       </c>
       <c r="B7" s="86" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="88" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D7" s="88" t="n">
         <f aca="false">IF(Circuit!B7, Circuit!B7 * Circuit!C7, "")</f>
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="E7" s="101" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F7" s="101" t="n">
         <f aca="false">IF(Circuit!B7, Circuit!B7 * Circuit!E7, "")</f>
-        <v>13</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3817,18 +3729,18 @@
         <v>1</v>
       </c>
       <c r="C8" s="88" t="n">
-        <v>0.1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="88" t="n">
         <f aca="false">IF(Circuit!B8, Circuit!B8 * Circuit!C8, "")</f>
-        <v>0.1</v>
+        <v>2</v>
       </c>
       <c r="E8" s="101" t="n">
-        <v>0.1</v>
+        <v>13</v>
       </c>
       <c r="F8" s="101" t="n">
         <f aca="false">IF(Circuit!B8, Circuit!B8 * Circuit!E8, "")</f>
-        <v>0.1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3836,21 +3748,21 @@
         <v>81</v>
       </c>
       <c r="B9" s="86" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C9" s="88" t="n">
         <v>0.1</v>
       </c>
       <c r="D9" s="88" t="n">
         <f aca="false">IF(Circuit!B9, Circuit!B9 * Circuit!C9, "")</f>
-        <v>0.7</v>
+        <v>0.1</v>
       </c>
       <c r="E9" s="101" t="n">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="F9" s="101" t="n">
         <f aca="false">IF(Circuit!B9, Circuit!B9 * Circuit!E9, "")</f>
-        <v>0.07</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3858,65 +3770,65 @@
         <v>82</v>
       </c>
       <c r="B10" s="86" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C10" s="88" t="n">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D10" s="88" t="n">
         <f aca="false">IF(Circuit!B10, Circuit!B10 * Circuit!C10, "")</f>
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="E10" s="101" t="n">
         <v>0.01</v>
       </c>
       <c r="F10" s="101" t="n">
         <f aca="false">IF(Circuit!B10, Circuit!B10 * Circuit!E10, "")</f>
-        <v>0.01</v>
+        <v>0.07</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="84" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" s="107" t="n">
+        <v>83</v>
+      </c>
+      <c r="B11" s="86" t="n">
         <v>1</v>
       </c>
       <c r="C11" s="88" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="D11" s="88" t="n">
         <f aca="false">IF(Circuit!B11, Circuit!B11 * Circuit!C11, "")</f>
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E11" s="101" t="n">
-        <v>30</v>
+        <v>0.01</v>
       </c>
       <c r="F11" s="101" t="n">
         <f aca="false">IF(Circuit!B11, Circuit!B11 * Circuit!E11, "")</f>
-        <v>30</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="84" t="s">
-        <v>83</v>
-      </c>
-      <c r="B12" s="86" t="n">
+        <v>63</v>
+      </c>
+      <c r="B12" s="107" t="n">
         <v>1</v>
       </c>
       <c r="C12" s="88" t="n">
-        <v>77</v>
+        <v>25</v>
       </c>
       <c r="D12" s="88" t="n">
         <f aca="false">IF(Circuit!B12, Circuit!B12 * Circuit!C12, "")</f>
-        <v>77</v>
+        <v>25</v>
       </c>
       <c r="E12" s="101" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F12" s="101" t="n">
         <f aca="false">IF(Circuit!B12, Circuit!B12 * Circuit!E12, "")</f>
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3924,21 +3836,21 @@
         <v>84</v>
       </c>
       <c r="B13" s="86" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C13" s="88" t="n">
-        <v>0.1</v>
+        <v>77</v>
       </c>
       <c r="D13" s="88" t="n">
         <f aca="false">IF(Circuit!B13, Circuit!B13 * Circuit!C13, "")</f>
-        <v>0.7</v>
+        <v>77</v>
       </c>
       <c r="E13" s="101" t="n">
-        <v>0.01</v>
+        <v>10</v>
       </c>
       <c r="F13" s="101" t="n">
         <f aca="false">IF(Circuit!B13, Circuit!B13 * Circuit!E13, "")</f>
-        <v>0.07</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3946,21 +3858,21 @@
         <v>85</v>
       </c>
       <c r="B14" s="86" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C14" s="88" t="n">
         <v>0.1</v>
       </c>
       <c r="D14" s="88" t="n">
         <f aca="false">IF(Circuit!B14, Circuit!B14 * Circuit!C14, "")</f>
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="E14" s="101" t="n">
         <v>0.01</v>
       </c>
       <c r="F14" s="101" t="n">
         <f aca="false">IF(Circuit!B14, Circuit!B14 * Circuit!E14, "")</f>
-        <v>0.1</v>
+        <v>0.07</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3968,87 +3880,87 @@
         <v>86</v>
       </c>
       <c r="B15" s="86" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C15" s="88" t="n">
         <v>0.1</v>
       </c>
       <c r="D15" s="88" t="n">
         <f aca="false">IF(Circuit!B15, Circuit!B15 * Circuit!C15, "")</f>
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="E15" s="101" t="n">
         <v>0.01</v>
       </c>
       <c r="F15" s="101" t="n">
         <f aca="false">IF(Circuit!B15, Circuit!B15 * Circuit!E15, "")</f>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="84" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="B16" s="86" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C16" s="88" t="n">
-        <v>124</v>
+        <v>0.1</v>
       </c>
       <c r="D16" s="88" t="n">
         <f aca="false">IF(Circuit!B16, Circuit!B16 * Circuit!C16, "")</f>
-        <v>372</v>
+        <v>0.4</v>
       </c>
       <c r="E16" s="101" t="n">
-        <v>50</v>
+        <v>0.01</v>
       </c>
       <c r="F16" s="101" t="n">
         <f aca="false">IF(Circuit!B16, Circuit!B16 * Circuit!E16, "")</f>
-        <v>150</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="84" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B17" s="86" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C17" s="88" t="n">
-        <v>47</v>
+        <v>124</v>
       </c>
       <c r="D17" s="88" t="n">
         <f aca="false">IF(Circuit!B17, Circuit!B17 * Circuit!C17, "")</f>
-        <v>47</v>
+        <v>372</v>
       </c>
       <c r="E17" s="101" t="n">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="F17" s="101" t="n">
         <f aca="false">IF(Circuit!B17, Circuit!B17 * Circuit!E17, "")</f>
-        <v>5</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="84" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="B18" s="86" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C18" s="88" t="n">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="D18" s="88" t="n">
         <f aca="false">IF(Circuit!B18, Circuit!B18 * Circuit!C18, "")</f>
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="E18" s="101" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F18" s="101" t="n">
         <f aca="false">IF(Circuit!B18, Circuit!B18 * Circuit!E18, "")</f>
-        <v>60</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4059,18 +3971,18 @@
         <v>3</v>
       </c>
       <c r="C19" s="88" t="n">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D19" s="88" t="n">
         <f aca="false">IF(Circuit!B19, Circuit!B19 * Circuit!C19, "")</f>
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="E19" s="101" t="n">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="F19" s="101" t="n">
         <f aca="false">IF(Circuit!B19, Circuit!B19 * Circuit!E19, "")</f>
-        <v>165</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4078,21 +3990,21 @@
         <v>89</v>
       </c>
       <c r="B20" s="86" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C20" s="88" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D20" s="88" t="n">
         <f aca="false">IF(Circuit!B20, Circuit!B20 * Circuit!C20, "")</f>
         <v>60</v>
       </c>
       <c r="E20" s="101" t="n">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="F20" s="101" t="n">
         <f aca="false">IF(Circuit!B20, Circuit!B20 * Circuit!E20, "")</f>
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4100,21 +4012,21 @@
         <v>90</v>
       </c>
       <c r="B21" s="86" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C21" s="88" t="n">
         <v>10</v>
       </c>
       <c r="D21" s="88" t="n">
         <f aca="false">IF(Circuit!B21, Circuit!B21 * Circuit!C21, "")</f>
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="E21" s="101" t="n">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="F21" s="101" t="n">
         <f aca="false">IF(Circuit!B21, Circuit!B21 * Circuit!E21, "")</f>
-        <v>96</v>
+        <v>168</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4122,21 +4034,21 @@
         <v>91</v>
       </c>
       <c r="B22" s="86" t="n">
+        <v>8</v>
+      </c>
+      <c r="C22" s="88" t="n">
         <v>10</v>
-      </c>
-      <c r="C22" s="88" t="n">
-        <v>1.1</v>
       </c>
       <c r="D22" s="88" t="n">
         <f aca="false">IF(Circuit!B22, Circuit!B22 * Circuit!C22, "")</f>
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="E22" s="101" t="n">
-        <v>0.1</v>
+        <v>12</v>
       </c>
       <c r="F22" s="101" t="n">
         <f aca="false">IF(Circuit!B22, Circuit!B22 * Circuit!E22, "")</f>
-        <v>1</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4144,31 +4056,43 @@
         <v>92</v>
       </c>
       <c r="B23" s="86" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C23" s="88" t="n">
         <v>1.1</v>
       </c>
       <c r="D23" s="88" t="n">
         <f aca="false">IF(Circuit!B23, Circuit!B23 * Circuit!C23, "")</f>
-        <v>2.2</v>
+        <v>11</v>
       </c>
       <c r="E23" s="101" t="n">
         <v>0.1</v>
       </c>
       <c r="F23" s="101" t="n">
         <f aca="false">IF(Circuit!B23, Circuit!B23 * Circuit!E23, "")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="84" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="86" t="n">
+        <v>2</v>
+      </c>
+      <c r="C24" s="88" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="D24" s="88" t="n">
+        <f aca="false">IF(Circuit!B24, Circuit!B24 * Circuit!C24, "")</f>
+        <v>2.2</v>
+      </c>
+      <c r="E24" s="101" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F24" s="101" t="n">
+        <f aca="false">IF(Circuit!B24, Circuit!B24 * Circuit!E24, "")</f>
         <v>0.2</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D24" s="88" t="str">
-        <f aca="false">IF(Circuit!B24, Circuit!B24 * Circuit!C24, "")</f>
-        <v/>
-      </c>
-      <c r="F24" s="101" t="str">
-        <f aca="false">IF(Circuit!B24, Circuit!B24 * Circuit!E24, "")</f>
-        <v/>
       </c>
     </row>
     <row r="25" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5931,14 +5855,23 @@
         <v/>
       </c>
     </row>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="201" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D201" s="88" t="str">
+        <f aca="false">IF(Circuit!B201, Circuit!B201 * Circuit!C201, "")</f>
+        <v/>
+      </c>
+      <c r="F201" s="101" t="str">
+        <f aca="false">IF(Circuit!B201, Circuit!B201 * Circuit!E201, "")</f>
+        <v/>
+      </c>
+    </row>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A3:F200"/>
+  <autoFilter ref="A3:F201"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -5955,13 +5888,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ210"/>
+  <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="19.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="19.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="84" width="45.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="86" width="16.81"/>
@@ -6003,27 +5936,27 @@
     </row>
     <row r="2" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="110" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B2" s="111" t="n">
         <f aca="true">IF(SUM(INDIRECT(Structură!B1)), SUM(INDIRECT(Structură!B1)), "")</f>
-        <v>245.8</v>
+        <v>589.4</v>
       </c>
       <c r="C2" s="112" t="n">
         <f aca="true">IF(SUM(INDIRECT(Structură!C1)), AVERAGE(INDIRECT(Structură!C1)), "")</f>
-        <v>5.14909090909091</v>
+        <v>1.26809523809524</v>
       </c>
       <c r="D2" s="112" t="n">
         <f aca="true">IF(SUM(INDIRECT(Structură!D1)), SUM(INDIRECT(Structură!D1)), "")</f>
-        <v>442.938</v>
+        <v>453.38</v>
       </c>
       <c r="E2" s="113" t="n">
         <f aca="true">IF(SUM(INDIRECT(Structură!E1)), AVERAGE(INDIRECT(Structură!E1)), "")</f>
-        <v>104.829545454545</v>
+        <v>8.91607142857143</v>
       </c>
       <c r="F2" s="113" t="n">
         <f aca="true">IF(SUM(INDIRECT(Structură!F1)), SUM(INDIRECT(Structură!F1)), "")</f>
-        <v>4170.75</v>
+        <v>3080.404</v>
       </c>
       <c r="G2" s="103"/>
     </row>
@@ -6049,486 +5982,480 @@
     </row>
     <row r="4" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="84" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B4" s="86" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C4" s="88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="88" t="n">
         <f aca="false">IF(Structură!B4, Structură!B4 * Structură!C4, "")</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E4" s="101" t="n">
-        <v>35</v>
+        <v>11.25</v>
       </c>
       <c r="F4" s="101" t="n">
         <f aca="false">IF(Structură!B4, Structură!B4 * Structură!E4, "")</f>
-        <v>140</v>
+        <v>11.25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="84" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B5" s="86" t="n">
-        <v>11</v>
+        <f aca="false"> 4 * (B7/2 - 2) + 4 * (B7 - 1) + 5</f>
+        <v>65</v>
       </c>
       <c r="C5" s="88" t="n">
         <v>1</v>
       </c>
       <c r="D5" s="88" t="n">
         <f aca="false">IF(Structură!B5, Structură!B5 * Structură!C5, "")</f>
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="E5" s="101" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F5" s="101" t="n">
         <f aca="false">IF(Structură!B5, Structură!B5 * Structură!E5, "")</f>
-        <v>154</v>
+        <v>975</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="84" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B6" s="86" t="n">
-        <v>68</v>
+        <v>4</v>
       </c>
       <c r="C6" s="88" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" s="88" t="n">
         <f aca="false">IF(Structură!B6, Structură!B6 * Structură!C6, "")</f>
-        <v>68</v>
+        <v>8</v>
       </c>
       <c r="E6" s="101" t="n">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="F6" s="101" t="n">
         <f aca="false">IF(Structură!B6, Structură!B6 * Structură!E6, "")</f>
-        <v>1156</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="84" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B7" s="86" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" s="88" t="n">
         <v>0.3</v>
       </c>
       <c r="D7" s="88" t="n">
         <f aca="false">IF(Structură!B7, Structură!B7 * Structură!C7, "")</f>
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="E7" s="101" t="n">
-        <v>22</v>
+        <v>12.5</v>
       </c>
       <c r="F7" s="101" t="n">
         <f aca="false">IF(Structură!B7, Structură!B7 * Structură!E7, "")</f>
-        <v>308</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="84" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B8" s="86" t="n">
         <v>4</v>
       </c>
       <c r="C8" s="88" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D8" s="88" t="n">
         <f aca="false">IF(Structură!B8, Structură!B8 * Structură!C8, "")</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E8" s="101" t="n">
-        <v>32</v>
+        <v>0.75</v>
       </c>
       <c r="F8" s="101" t="n">
         <f aca="false">IF(Structură!B8, Structură!B8 * Structură!E8, "")</f>
-        <v>128</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="84" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B9" s="86" t="n">
-        <v>4</v>
+        <f aca="false"> 5 * B7</f>
+        <v>60</v>
       </c>
       <c r="C9" s="88" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D9" s="88" t="n">
         <f aca="false">IF(Structură!B9, Structură!B9 * Structură!C9, "")</f>
-        <v>8</v>
+        <v>180</v>
       </c>
       <c r="E9" s="101" t="n">
-        <v>37.5</v>
+        <v>10.75</v>
       </c>
       <c r="F9" s="101" t="n">
         <f aca="false">IF(Structură!B9, Structură!B9 * Structură!E9, "")</f>
-        <v>150</v>
+        <v>645</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="84" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B10" s="86" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C10" s="88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10" s="88" t="n">
         <f aca="false">IF(Structură!B10, Structură!B10 * Structură!C10, "")</f>
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E10" s="101" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F10" s="101" t="n">
         <f aca="false">IF(Structură!B10, Structură!B10 * Structură!E10, "")</f>
-        <v>60</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="114" t="s">
-        <v>101</v>
+      <c r="A11" s="84" t="s">
+        <v>102</v>
       </c>
       <c r="B11" s="86" t="n">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="C11" s="88" t="n">
         <v>2</v>
       </c>
       <c r="D11" s="88" t="n">
         <f aca="false">IF(Structură!B11, Structură!B11 * Structură!C11, "")</f>
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="E11" s="101" t="n">
-        <v>9</v>
+        <v>28.57</v>
       </c>
       <c r="F11" s="101" t="n">
         <f aca="false">IF(Structură!B11, Structură!B11 * Structură!E11, "")</f>
-        <v>90</v>
+        <v>771.39</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="84" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B12" s="86" t="n">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="C12" s="88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D12" s="88" t="n">
         <f aca="false">IF(Structură!B12, Structură!B12 * Structură!C12, "")</f>
-        <v>165</v>
+        <v>28</v>
       </c>
       <c r="E12" s="101" t="n">
-        <v>11.25</v>
+        <v>5</v>
       </c>
       <c r="F12" s="101" t="n">
         <f aca="false">IF(Structură!B12, Structură!B12 * Structură!E12, "")</f>
-        <v>618.75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="114" t="s">
-        <v>101</v>
+      <c r="A13" s="84" t="s">
+        <v>104</v>
       </c>
       <c r="B13" s="86" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C13" s="88" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D13" s="88" t="n">
         <f aca="false">IF(Structură!B13, Structură!B13 * Structură!C13, "")</f>
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="E13" s="101" t="n">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="F13" s="101" t="n">
         <f aca="false">IF(Structură!B13, Structură!B13 * Structură!E13, "")</f>
-        <v>114</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="84" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B14" s="86" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" s="88" t="n">
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="D14" s="88" t="n">
         <f aca="false">IF(Structură!B14, Structură!B14 * Structură!C14, "")</f>
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="E14" s="101" t="n">
-        <v>11</v>
+        <v>3.5</v>
       </c>
       <c r="F14" s="101" t="n">
         <f aca="false">IF(Structură!B14, Structură!B14 * Structură!E14, "")</f>
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="84" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B15" s="86" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C15" s="88" t="n">
-        <v>2</v>
+        <v>2.45</v>
       </c>
       <c r="D15" s="88" t="n">
         <f aca="false">IF(Structură!B15, Structură!B15 * Structură!C15, "")</f>
-        <v>28</v>
+        <v>4.9</v>
       </c>
       <c r="E15" s="101" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F15" s="101" t="n">
         <f aca="false">IF(Structură!B15, Structură!B15 * Structură!E15, "")</f>
-        <v>280</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="84" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B16" s="86" t="n">
-        <v>12</v>
+        <v>0.4</v>
       </c>
       <c r="C16" s="88" t="n">
-        <v>1.75</v>
+        <v>0.25</v>
       </c>
       <c r="D16" s="88" t="n">
         <f aca="false">IF(Structură!B16, Structură!B16 * Structură!C16, "")</f>
-        <v>21</v>
+        <v>0.1</v>
       </c>
       <c r="E16" s="101" t="n">
-        <v>3.5</v>
+        <v>0.06</v>
       </c>
       <c r="F16" s="101" t="n">
         <f aca="false">IF(Structură!B16, Structură!B16 * Structură!E16, "")</f>
-        <v>42</v>
+        <v>0.024</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="114" t="s">
-        <v>105</v>
+      <c r="A17" s="84" t="s">
+        <v>108</v>
       </c>
       <c r="B17" s="86" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C17" s="88" t="n">
-        <v>2.45</v>
-      </c>
-      <c r="D17" s="88" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="D17" s="88" t="str">
         <f aca="false">IF(Structură!B17, Structură!B17 * Structură!C17, "")</f>
-        <v>19.6</v>
+        <v/>
       </c>
       <c r="E17" s="101" t="n">
-        <v>5</v>
-      </c>
-      <c r="F17" s="101" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="F17" s="101" t="str">
         <f aca="false">IF(Structură!B17, Structură!B17 * Structură!E17, "")</f>
-        <v>40</v>
+        <v/>
       </c>
     </row>
     <row r="18" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="84" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B18" s="86" t="n">
-        <v>0.4</v>
+        <f aca="false">B19+B20+B21+8*B7</f>
+        <v>240</v>
       </c>
       <c r="C18" s="88" t="n">
-        <v>37.9</v>
+        <v>0.2</v>
       </c>
       <c r="D18" s="88" t="n">
         <f aca="false">IF(Structură!B18, Structură!B18 * Structură!C18, "")</f>
-        <v>15.16</v>
-      </c>
-      <c r="E18" s="101" t="n">
-        <v>1000</v>
+        <v>48</v>
+      </c>
+      <c r="E18" s="114" t="n">
+        <v>0.03</v>
       </c>
       <c r="F18" s="101" t="n">
         <f aca="false">IF(Structură!B18, Structură!B18 * Structură!E18, "")</f>
-        <v>400</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="84" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B19" s="86" t="n">
-        <v>0</v>
+        <f aca="false">B7 * 4</f>
+        <v>48</v>
       </c>
       <c r="C19" s="88" t="n">
-        <v>0.49</v>
-      </c>
-      <c r="D19" s="88" t="str">
+        <v>0.2</v>
+      </c>
+      <c r="D19" s="88" t="n">
         <f aca="false">IF(Structură!B19, Structură!B19 * Structură!C19, "")</f>
-        <v/>
+        <v>9.6</v>
       </c>
       <c r="E19" s="101" t="n">
-        <v>1</v>
-      </c>
-      <c r="F19" s="101" t="str">
+        <v>0.03</v>
+      </c>
+      <c r="F19" s="101" t="n">
         <f aca="false">IF(Structură!B19, Structură!B19 * Structură!E19, "")</f>
-        <v/>
+        <v>1.44</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="84" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B20" s="86" t="n">
-        <v>4</v>
+        <f aca="false">B7 * 4</f>
+        <v>48</v>
       </c>
       <c r="C20" s="88" t="n">
-        <v>0.29</v>
+        <v>0.2</v>
       </c>
       <c r="D20" s="88" t="n">
         <f aca="false">IF(Structură!B20, Structură!B20 * Structură!C20, "")</f>
-        <v>1.16</v>
+        <v>9.6</v>
       </c>
       <c r="E20" s="101" t="n">
-        <v>1</v>
+        <v>0.0625</v>
       </c>
       <c r="F20" s="101" t="n">
         <f aca="false">IF(Structură!B20, Structură!B20 * Structură!E20, "")</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="84" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B21" s="86" t="n">
-        <v>0.4</v>
+        <f aca="false">B7 * 4</f>
+        <v>48</v>
       </c>
       <c r="C21" s="88" t="n">
-        <v>42.12</v>
+        <v>0.25</v>
       </c>
       <c r="D21" s="88" t="n">
         <f aca="false">IF(Structură!B21, Structură!B21 * Structură!C21, "")</f>
-        <v>16.848</v>
+        <v>12</v>
       </c>
       <c r="E21" s="101" t="n">
-        <v>1000</v>
+        <v>0.125</v>
       </c>
       <c r="F21" s="101" t="n">
         <f aca="false">IF(Structură!B21, Structură!B21 * Structură!E21, "")</f>
-        <v>400</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="114" t="s">
-        <v>110</v>
+      <c r="A22" s="84" t="s">
+        <v>113</v>
       </c>
       <c r="B22" s="86" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C22" s="88" t="n">
-        <v>0.49</v>
+        <v>0.25</v>
       </c>
       <c r="D22" s="88" t="n">
         <f aca="false">IF(Structură!B22, Structură!B22 * Structură!C22, "")</f>
-        <v>4.41</v>
+        <v>0.5</v>
       </c>
       <c r="E22" s="101" t="n">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="F22" s="101" t="n">
         <f aca="false">IF(Structură!B22, Structură!B22 * Structură!E22, "")</f>
-        <v>9</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="114" t="s">
-        <v>111</v>
+      <c r="A23" s="84" t="s">
+        <v>114</v>
       </c>
       <c r="B23" s="86" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C23" s="88" t="n">
         <v>0.29</v>
       </c>
       <c r="D23" s="88" t="n">
         <f aca="false">IF(Structură!B23, Structură!B23 * Structură!C23, "")</f>
-        <v>1.16</v>
+        <v>0.58</v>
       </c>
       <c r="E23" s="101" t="n">
-        <v>1</v>
+        <v>0.35</v>
       </c>
       <c r="F23" s="101" t="n">
         <f aca="false">IF(Structură!B23, Structură!B23 * Structură!E23, "")</f>
-        <v>4</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="114" t="s">
-        <v>112</v>
+      <c r="A24" s="84" t="s">
+        <v>115</v>
       </c>
       <c r="B24" s="86" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C24" s="88" t="n">
-        <v>0.2</v>
+        <v>3</v>
       </c>
       <c r="D24" s="88" t="n">
         <f aca="false">IF(Structură!B24, Structură!B24 * Structură!C24, "")</f>
-        <v>2.4</v>
+        <v>3</v>
       </c>
       <c r="E24" s="101" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F24" s="101" t="n">
         <f aca="false">IF(Structură!B24, Structură!B24 * Structură!E24, "")</f>
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="84" t="s">
-        <v>113</v>
-      </c>
-      <c r="B25" s="86" t="n">
-        <v>1</v>
-      </c>
-      <c r="C25" s="88" t="n">
-        <v>3</v>
-      </c>
-      <c r="D25" s="88" t="n">
+      <c r="D25" s="88" t="str">
         <f aca="false">IF(Structură!B25, Structură!B25 * Structură!C25, "")</f>
-        <v>3</v>
-      </c>
-      <c r="E25" s="101" t="n">
-        <v>50</v>
-      </c>
-      <c r="F25" s="101" t="n">
+        <v/>
+      </c>
+      <c r="F25" s="101" t="str">
         <f aca="false">IF(Structură!B25, Structură!B25 * Structură!E25, "")</f>
-        <v>50</v>
+        <v/>
       </c>
     </row>
     <row r="26" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8371,18 +8298,9 @@
         <v/>
       </c>
     </row>
-    <row r="210" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D210" s="88" t="str">
-        <f aca="false">IF(Structură!B210, Structură!B210 * Structură!C210, "")</f>
-        <v/>
-      </c>
-      <c r="F210" s="101" t="str">
-        <f aca="false">IF(Structură!B210, Structură!B210 * Structură!E210, "")</f>
-        <v/>
-      </c>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A3:F210"/>
+  <autoFilter ref="A3:F209"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -8402,10 +8320,10 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="19.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="19.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="84" width="30.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="86" width="16.81"/>
@@ -8447,27 +8365,27 @@
     </row>
     <row r="2" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="117" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B2" s="118" t="n">
         <f aca="true">IF(SUM(INDIRECT(Carcasă!B1)), SUM(INDIRECT(Carcasă!B1)), "")</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="119" t="n">
         <f aca="true">IF(SUM(INDIRECT(Carcasă!C1)), AVERAGE(INDIRECT(Carcasă!C1)), "")</f>
-        <v>11</v>
+        <v>30.5</v>
       </c>
       <c r="D2" s="119" t="n">
         <f aca="true">IF(SUM(INDIRECT(Carcasă!D1)), SUM(INDIRECT(Carcasă!D1)), "")</f>
-        <v>94</v>
+        <v>190</v>
       </c>
       <c r="E2" s="120" t="n">
         <f aca="true">IF(SUM(INDIRECT(Carcasă!E1)), AVERAGE(INDIRECT(Carcasă!E1)), "")</f>
-        <v>125</v>
+        <v>201.25</v>
       </c>
       <c r="F2" s="120" t="n">
         <f aca="true">IF(SUM(INDIRECT(Carcasă!F1)), SUM(INDIRECT(Carcasă!F1)), "")</f>
-        <v>1300</v>
+        <v>1365</v>
       </c>
       <c r="G2" s="103"/>
     </row>
@@ -8493,29 +8411,29 @@
     </row>
     <row r="4" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="84" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B4" s="86" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="88" t="n">
-        <v>21</v>
+        <v>60</v>
       </c>
       <c r="D4" s="88" t="n">
         <f aca="false">IF(Carcasă!B4, Carcasă!B4 * Carcasă!C4, "")</f>
-        <v>84</v>
+        <v>180</v>
       </c>
       <c r="E4" s="101" t="n">
-        <v>200</v>
+        <v>380</v>
       </c>
       <c r="F4" s="101" t="n">
         <f aca="false">IF(Carcasă!B4, Carcasă!B4 * Carcasă!E4, "")</f>
-        <v>800</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="84" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B5" s="86" t="n">
         <v>10</v>
@@ -8528,11 +8446,11 @@
         <v>10</v>
       </c>
       <c r="E5" s="101" t="n">
-        <v>50</v>
+        <v>22.5</v>
       </c>
       <c r="F5" s="101" t="n">
         <f aca="false">IF(Carcasă!B5, Carcasă!B5 * Carcasă!E5, "")</f>
-        <v>500</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10464,7 +10382,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="19.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="19.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="84" width="55.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="86" width="16.81"/>
@@ -10506,7 +10424,7 @@
     </row>
     <row r="2" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="123" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B2" s="124" t="n">
         <f aca="true">IF(SUM(INDIRECT(Telecomandă!B1)), SUM(INDIRECT(Telecomandă!B1)), "")</f>
@@ -10552,7 +10470,7 @@
     </row>
     <row r="4" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="84" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B4" s="86" t="n">
         <v>1</v>
@@ -10596,7 +10514,7 @@
     </row>
     <row r="6" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="84" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B6" s="86" t="n">
         <v>1</v>
@@ -10618,7 +10536,7 @@
     </row>
     <row r="7" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="84" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B7" s="86" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
Update documentation, schematic and readme
</commit_message>
<xml_diff>
--- a/documents/Documentation.xlsx
+++ b/documents/Documentation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Centralizare" sheetId="1" state="visible" r:id="rId2"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="119">
   <si>
     <t xml:space="preserve">Componentă</t>
   </si>
@@ -116,10 +116,10 @@
     <t xml:space="preserve">Adâncime maximă</t>
   </si>
   <si>
-    <t xml:space="preserve">Compartiment 1 – Elice</t>
+    <t xml:space="preserve">Compartiment 1 – Provă</t>
   </si>
   <si>
-    <t xml:space="preserve">Compartiment 2 – Provă</t>
+    <t xml:space="preserve">Compartiment 2</t>
   </si>
   <si>
     <t xml:space="preserve">Compartiment 3</t>
@@ -134,16 +134,16 @@
     <t xml:space="preserve">Compartiment 6</t>
   </si>
   <si>
-    <t xml:space="preserve">Compartiment 7</t>
+    <t xml:space="preserve">Compartiment 7 – Pupă</t>
   </si>
   <si>
-    <t xml:space="preserve">Compartiment 8 – Pupă</t>
+    <t xml:space="preserve">Compartiment 8 – Corpul de navigație</t>
   </si>
   <si>
-    <t xml:space="preserve">Compartiment 9 – Corpul de navigație</t>
+    <t xml:space="preserve">Elice</t>
   </si>
   <si>
-    <t xml:space="preserve">Cârmă</t>
+    <t xml:space="preserve">Cârme</t>
   </si>
   <si>
     <t xml:space="preserve">Plane de scufundare față</t>
@@ -344,7 +344,7 @@
     <t xml:space="preserve">Cornier Negru cu Șuruburi pentru Motoarele N20 </t>
   </si>
   <si>
-    <t xml:space="preserve">Bară cilindrică hot glue 11x300 mm</t>
+    <t xml:space="preserve">Silicon 300ml negru</t>
   </si>
   <si>
     <t xml:space="preserve">Magnet adeziv disc 12 mm</t>
@@ -368,28 +368,25 @@
     <t xml:space="preserve">Șaibă M3</t>
   </si>
   <si>
-    <t xml:space="preserve">Șuruburi M3  4 mm</t>
+    <t xml:space="preserve">Șuruburi M3  8 mm cap înecat</t>
   </si>
   <si>
-    <t xml:space="preserve">Șuruburi M3  8 mm</t>
+    <t xml:space="preserve">Șuruburi M3  8 mm cap rotund</t>
   </si>
   <si>
-    <t xml:space="preserve">Șuruburi M3 16 mm</t>
+    <t xml:space="preserve">Șuruburi M3 16 mm cap înecat</t>
   </si>
   <si>
-    <t xml:space="preserve">Șuruburi M3 25 mm</t>
+    <t xml:space="preserve">Șuruburi M3 25 mm cap rotund</t>
   </si>
   <si>
-    <t xml:space="preserve">Șuruburi M3 45 mm</t>
+    <t xml:space="preserve">Șuruburi M3 45 mm cap rotund</t>
   </si>
   <si>
     <t xml:space="preserve">Tijă filetată M3 1 m</t>
   </si>
   <si>
     <t xml:space="preserve">Carcasă</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Silicon 300ml</t>
   </si>
   <si>
     <t xml:space="preserve">PET 1.5 L</t>
@@ -424,7 +421,7 @@
     <numFmt numFmtId="182" formatCode="@"/>
     <numFmt numFmtId="183" formatCode="#,##0.00\ [$RON];\-#,##0.00\ [$RON]"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -535,12 +532,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1235,6 +1226,10 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="182" fontId="13" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1251,15 +1246,11 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="17" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="12" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="181" fontId="18" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="181" fontId="17" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1279,11 +1270,11 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="181" fontId="19" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="181" fontId="18" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1420,7 +1411,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="18.38"/>
@@ -1526,7 +1517,7 @@
       </c>
       <c r="M2" s="25" t="n">
         <f aca="false">C5 / 1000</f>
-        <v>6.209994</v>
+        <v>5.90128</v>
       </c>
       <c r="N2" s="25" t="n">
         <f aca="false">J2 * K2</f>
@@ -1534,7 +1525,7 @@
       </c>
       <c r="O2" s="26" t="n">
         <f aca="false">L2 * M2 / N2</f>
-        <v>0.0790514235439748</v>
+        <v>0.0751215838101595</v>
       </c>
       <c r="AMB2" s="0"/>
       <c r="AMC2" s="0"/>
@@ -1553,11 +1544,11 @@
       </c>
       <c r="B3" s="28" t="n">
         <f aca="true">INDIRECT(ADDRESS(Centralizare!$D$2, Centralizare!$D$3, 1, 1, Centralizare!$A3), 1)</f>
-        <v>453.38</v>
+        <v>858</v>
       </c>
       <c r="C3" s="29" t="n">
         <f aca="true">INDIRECT(ADDRESS(Centralizare!$D$2, Centralizare!$D$4, 1, 1, Centralizare!$A3), 1)</f>
-        <v>3080.404</v>
+        <v>3011.69</v>
       </c>
       <c r="D3" s="14" t="n">
         <v>4</v>
@@ -1597,7 +1588,7 @@
       </c>
       <c r="C4" s="32" t="n">
         <f aca="true">INDIRECT(ADDRESS(Centralizare!$D$2, Centralizare!$D$4, 1, 1, Centralizare!$A4), 1)</f>
-        <v>1365</v>
+        <v>1125</v>
       </c>
       <c r="D4" s="14" t="n">
         <v>6</v>
@@ -1632,11 +1623,11 @@
       </c>
       <c r="B5" s="34" t="n">
         <f aca="false">IF(SUM(B2:B4), SUM(B2:B4), "")</f>
-        <v>2017.72</v>
+        <v>2422.34</v>
       </c>
       <c r="C5" s="35" t="n">
         <f aca="false">IF(SUM(C2:C3), SUM(C2:C4), "")</f>
-        <v>6209.994</v>
+        <v>5901.28</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="19" t="n">
@@ -1683,11 +1674,11 @@
       </c>
       <c r="B7" s="40" t="n">
         <f aca="false">IF(SUM(B5:B6), SUM(B5:B6), "")</f>
-        <v>2073.72</v>
+        <v>2478.34</v>
       </c>
       <c r="C7" s="41" t="n">
         <f aca="false">IF(SUM(C5:C6), SUM(C5:C6), "")</f>
-        <v>6334.994</v>
+        <v>6026.28</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1713,11 +1704,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="15.56"/>
@@ -1770,29 +1761,29 @@
         <v>26</v>
       </c>
       <c r="B2" s="26" t="n">
-        <v>0.07</v>
+        <v>0.1</v>
       </c>
       <c r="C2" s="26" t="n">
-        <v>0.07</v>
+        <v>0.1</v>
       </c>
       <c r="D2" s="43" t="n">
         <f aca="false">PI() * C2 / 2 * B2</f>
-        <v>0.007696902001295</v>
+        <v>0.015707963267949</v>
       </c>
       <c r="E2" s="22" t="n">
-        <f aca="false">PI() * POWER(C2 / 2, 2) * B2</f>
-        <v>0.000269391570045325</v>
+        <f aca="false">PI() * POWER(C2 / 2, 2) * B2 * 0.75</f>
+        <v>0.000589048622548086</v>
       </c>
       <c r="F2" s="43" t="n">
         <f aca="false">B2 * C2</f>
-        <v>0.0049</v>
+        <v>0.01</v>
       </c>
       <c r="G2" s="44" t="n">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="H2" s="45" t="n">
         <f aca="false">G2/Centralizare!$K$2/F2</f>
-        <v>10.2040816326531</v>
+        <v>12</v>
       </c>
       <c r="ALY2" s="0"/>
       <c r="ALZ2" s="0"/>
@@ -1812,29 +1803,30 @@
         <v>27</v>
       </c>
       <c r="B3" s="26" t="n">
-        <v>0.1</v>
+        <v>0.13</v>
       </c>
       <c r="C3" s="26" t="n">
+        <f aca="false">C2</f>
         <v>0.1</v>
       </c>
       <c r="D3" s="43" t="n">
         <f aca="false">PI() * C3 / 2 * B3</f>
-        <v>0.015707963267949</v>
+        <v>0.0204203522483337</v>
       </c>
       <c r="E3" s="22" t="n">
-        <f aca="false">PI() * POWER(C3 / 2, 2) * B3 * 0.75</f>
-        <v>0.000589048622548086</v>
+        <f aca="false">PI() * POWER(C3 / 2, 2) * B3</f>
+        <v>0.00102101761241668</v>
       </c>
       <c r="F3" s="43" t="n">
         <f aca="false">B3 * C3</f>
-        <v>0.01</v>
+        <v>0.013</v>
       </c>
       <c r="G3" s="44" t="n">
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="H3" s="45" t="n">
         <f aca="false">G3/Centralizare!$K$2/F3</f>
-        <v>12</v>
+        <v>12.3076923076923</v>
       </c>
       <c r="ALY3" s="0"/>
       <c r="ALZ3" s="0"/>
@@ -1857,7 +1849,7 @@
         <v>0.13</v>
       </c>
       <c r="C4" s="26" t="n">
-        <f aca="false">C3</f>
+        <f aca="false">C2</f>
         <v>0.1</v>
       </c>
       <c r="D4" s="43" t="n">
@@ -1897,30 +1889,30 @@
         <v>29</v>
       </c>
       <c r="B5" s="26" t="n">
-        <v>0.13</v>
+        <v>0.25</v>
       </c>
       <c r="C5" s="26" t="n">
-        <f aca="false">C3</f>
+        <f aca="false">C2</f>
         <v>0.1</v>
       </c>
       <c r="D5" s="43" t="n">
         <f aca="false">PI() * C5 / 2 * B5</f>
-        <v>0.0204203522483337</v>
+        <v>0.0392699081698724</v>
       </c>
       <c r="E5" s="22" t="n">
         <f aca="false">PI() * POWER(C5 / 2, 2) * B5</f>
-        <v>0.00102101761241668</v>
+        <v>0.00196349540849362</v>
       </c>
       <c r="F5" s="43" t="n">
         <f aca="false">B5 * C5</f>
-        <v>0.013</v>
+        <v>0.025</v>
       </c>
       <c r="G5" s="44" t="n">
-        <v>160</v>
+        <v>250</v>
       </c>
       <c r="H5" s="45" t="n">
         <f aca="false">G5/Centralizare!$K$2/F5</f>
-        <v>12.3076923076923</v>
+        <v>10</v>
       </c>
       <c r="ALY5" s="0"/>
       <c r="ALZ5" s="0"/>
@@ -1940,30 +1932,30 @@
         <v>30</v>
       </c>
       <c r="B6" s="26" t="n">
-        <v>0.25</v>
+        <v>0.13</v>
       </c>
       <c r="C6" s="26" t="n">
-        <f aca="false">C3</f>
+        <f aca="false">C2</f>
         <v>0.1</v>
       </c>
       <c r="D6" s="43" t="n">
         <f aca="false">PI() * C6 / 2 * B6</f>
-        <v>0.0392699081698724</v>
+        <v>0.0204203522483337</v>
       </c>
       <c r="E6" s="22" t="n">
         <f aca="false">PI() * POWER(C6 / 2, 2) * B6</f>
-        <v>0.00196349540849362</v>
+        <v>0.00102101761241668</v>
       </c>
       <c r="F6" s="43" t="n">
         <f aca="false">B6 * C6</f>
-        <v>0.025</v>
+        <v>0.013</v>
       </c>
       <c r="G6" s="44" t="n">
-        <v>250</v>
+        <v>160</v>
       </c>
       <c r="H6" s="45" t="n">
         <f aca="false">G6/Centralizare!$K$2/F6</f>
-        <v>10</v>
+        <v>12.3076923076923</v>
       </c>
       <c r="ALY6" s="0"/>
       <c r="ALZ6" s="0"/>
@@ -1986,7 +1978,7 @@
         <v>0.13</v>
       </c>
       <c r="C7" s="26" t="n">
-        <f aca="false">C3</f>
+        <f aca="false">C2</f>
         <v>0.1</v>
       </c>
       <c r="D7" s="43" t="n">
@@ -2002,11 +1994,11 @@
         <v>0.013</v>
       </c>
       <c r="G7" s="44" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="H7" s="45" t="n">
         <f aca="false">G7/Centralizare!$K$2/F7</f>
-        <v>12.3076923076923</v>
+        <v>15.3846153846154</v>
       </c>
       <c r="ALY7" s="0"/>
       <c r="ALZ7" s="0"/>
@@ -2026,30 +2018,30 @@
         <v>32</v>
       </c>
       <c r="B8" s="26" t="n">
-        <v>0.13</v>
+        <v>0.085</v>
       </c>
       <c r="C8" s="26" t="n">
-        <f aca="false">C3</f>
+        <f aca="false">C2</f>
         <v>0.1</v>
       </c>
       <c r="D8" s="43" t="n">
-        <f aca="false">PI() * C8 / 2 * B8</f>
-        <v>0.0204203522483337</v>
+        <f aca="false">2 * PI() * C8 * B8</f>
+        <v>0.0534070751110265</v>
       </c>
       <c r="E8" s="22" t="n">
-        <f aca="false">PI() * POWER(C8 / 2, 2) * B8</f>
-        <v>0.00102101761241668</v>
+        <f aca="false">PI() / 12 * POWER(C8 / 2, 2) * B8</f>
+        <v>5.56323699073193E-005</v>
       </c>
       <c r="F8" s="43" t="n">
         <f aca="false">B8 * C8</f>
-        <v>0.013</v>
+        <v>0.0085</v>
       </c>
       <c r="G8" s="44" t="n">
-        <v>200</v>
+        <v>85</v>
       </c>
       <c r="H8" s="45" t="n">
         <f aca="false">G8/Centralizare!$K$2/F8</f>
-        <v>15.3846153846154</v>
+        <v>10</v>
       </c>
       <c r="ALY8" s="0"/>
       <c r="ALZ8" s="0"/>
@@ -2069,30 +2061,29 @@
         <v>33</v>
       </c>
       <c r="B9" s="26" t="n">
-        <v>0.085</v>
+        <v>0.2</v>
       </c>
       <c r="C9" s="26" t="n">
-        <f aca="false">C3</f>
-        <v>0.1</v>
+        <v>0.07</v>
       </c>
       <c r="D9" s="43" t="n">
-        <f aca="false">2 * PI() * C9 * B9</f>
-        <v>0.0534070751110265</v>
+        <f aca="false">PI() * C9 / 2 * B9</f>
+        <v>0.0219911485751286</v>
       </c>
       <c r="E9" s="22" t="n">
-        <f aca="false">PI() / 12 * POWER(C9 / 2, 2) * B9</f>
-        <v>5.56323699073193E-005</v>
+        <f aca="false">B9 * C9 * 0.06</f>
+        <v>0.00084</v>
       </c>
       <c r="F9" s="43" t="n">
         <f aca="false">B9 * C9</f>
-        <v>0.0085</v>
+        <v>0.014</v>
       </c>
       <c r="G9" s="44" t="n">
-        <v>85</v>
+        <v>150</v>
       </c>
       <c r="H9" s="45" t="n">
         <f aca="false">G9/Centralizare!$K$2/F9</f>
-        <v>10</v>
+        <v>10.7142857142857</v>
       </c>
       <c r="ALY9" s="0"/>
       <c r="ALZ9" s="0"/>
@@ -2112,29 +2103,29 @@
         <v>34</v>
       </c>
       <c r="B10" s="26" t="n">
-        <v>0.2</v>
+        <v>0.07</v>
       </c>
       <c r="C10" s="26" t="n">
         <v>0.07</v>
       </c>
       <c r="D10" s="43" t="n">
         <f aca="false">PI() * C10 / 2 * B10</f>
-        <v>0.0219911485751286</v>
+        <v>0.007696902001295</v>
       </c>
       <c r="E10" s="22" t="n">
-        <f aca="false">B10 * C10 * 0.06</f>
-        <v>0.00084</v>
+        <f aca="false">PI() * POWER(C10 / 2, 2) * B10</f>
+        <v>0.000269391570045325</v>
       </c>
       <c r="F10" s="43" t="n">
         <f aca="false">B10 * C10</f>
-        <v>0.014</v>
+        <v>0.0049</v>
       </c>
       <c r="G10" s="44" t="n">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="H10" s="45" t="n">
         <f aca="false">G10/Centralizare!$K$2/F10</f>
-        <v>10.7142857142857</v>
+        <v>10.2040816326531</v>
       </c>
       <c r="ALY10" s="0"/>
       <c r="ALZ10" s="0"/>
@@ -2278,11 +2269,11 @@
     <row r="14" s="15" customFormat="true" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="20"/>
       <c r="B14" s="26" t="n">
-        <f aca="false">SUM(B2:B9)</f>
-        <v>1.025</v>
+        <f aca="false">SUM(B2:B8)</f>
+        <v>0.955</v>
       </c>
       <c r="C14" s="26" t="n">
-        <f aca="false">C3 + 2 * C12</f>
+        <f aca="false">C2 + 2 * C12</f>
         <v>0.16</v>
       </c>
       <c r="D14" s="43"/>
@@ -2333,7 +2324,7 @@
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="19.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="19.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="46" width="25.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="47" width="10.19"/>
@@ -3192,7 +3183,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="84" width="50.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="85" width="21.95"/>
@@ -3543,11 +3534,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="19.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="19.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="84" width="55.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="86" width="16.81"/>
@@ -5890,11 +5881,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="19.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="19.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="84" width="45.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="86" width="16.81"/>
@@ -5932,31 +5923,34 @@
       <c r="H1" s="93" t="n">
         <v>100</v>
       </c>
+      <c r="I1" s="110" t="n">
+        <v>12</v>
+      </c>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="110" t="s">
+      <c r="A2" s="111" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="111" t="n">
+      <c r="B2" s="112" t="n">
         <f aca="true">IF(SUM(INDIRECT(Structură!B1)), SUM(INDIRECT(Structură!B1)), "")</f>
-        <v>589.4</v>
-      </c>
-      <c r="C2" s="112" t="n">
+        <v>1669</v>
+      </c>
+      <c r="C2" s="113" t="n">
         <f aca="true">IF(SUM(INDIRECT(Structură!C1)), AVERAGE(INDIRECT(Structură!C1)), "")</f>
-        <v>1.26809523809524</v>
-      </c>
-      <c r="D2" s="112" t="n">
+        <v>4.03</v>
+      </c>
+      <c r="D2" s="113" t="n">
         <f aca="true">IF(SUM(INDIRECT(Structură!D1)), SUM(INDIRECT(Structură!D1)), "")</f>
-        <v>453.38</v>
-      </c>
-      <c r="E2" s="113" t="n">
+        <v>858</v>
+      </c>
+      <c r="E2" s="114" t="n">
         <f aca="true">IF(SUM(INDIRECT(Structură!E1)), AVERAGE(INDIRECT(Structură!E1)), "")</f>
-        <v>8.91607142857143</v>
-      </c>
-      <c r="F2" s="113" t="n">
+        <v>21.6047619047619</v>
+      </c>
+      <c r="F2" s="114" t="n">
         <f aca="true">IF(SUM(INDIRECT(Structură!F1)), SUM(INDIRECT(Structură!F1)), "")</f>
-        <v>3080.404</v>
+        <v>3011.69</v>
       </c>
       <c r="G2" s="103"/>
     </row>
@@ -5985,21 +5979,21 @@
         <v>95</v>
       </c>
       <c r="B4" s="86" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="88" t="n">
         <v>1</v>
       </c>
-      <c r="D4" s="88" t="n">
+      <c r="D4" s="88" t="str">
         <f aca="false">IF(Structură!B4, Structură!B4 * Structură!C4, "")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="E4" s="101" t="n">
         <v>11.25</v>
       </c>
-      <c r="F4" s="101" t="n">
+      <c r="F4" s="101" t="str">
         <f aca="false">IF(Structură!B4, Structură!B4 * Structură!E4, "")</f>
-        <v>11.25</v>
+        <v/>
       </c>
     </row>
     <row r="5" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6007,22 +6001,22 @@
         <v>96</v>
       </c>
       <c r="B5" s="86" t="n">
-        <f aca="false"> 4 * (B7/2 - 2) + 4 * (B7 - 1) + 5</f>
-        <v>65</v>
+        <f aca="false">3 * $I$1</f>
+        <v>36</v>
       </c>
       <c r="C5" s="88" t="n">
         <v>1</v>
       </c>
       <c r="D5" s="88" t="n">
         <f aca="false">IF(Structură!B5, Structură!B5 * Structură!C5, "")</f>
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="E5" s="101" t="n">
         <v>15</v>
       </c>
       <c r="F5" s="101" t="n">
         <f aca="false">IF(Structură!B5, Structură!B5 * Structură!E5, "")</f>
-        <v>975</v>
+        <v>540</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6052,6 +6046,7 @@
         <v>98</v>
       </c>
       <c r="B7" s="86" t="n">
+        <f aca="false">$I$1</f>
         <v>12</v>
       </c>
       <c r="C7" s="88" t="n">
@@ -6096,22 +6091,22 @@
         <v>100</v>
       </c>
       <c r="B9" s="86" t="n">
-        <f aca="false"> 5 * B7</f>
-        <v>60</v>
+        <f aca="false">6 * $I$1</f>
+        <v>72</v>
       </c>
       <c r="C9" s="88" t="n">
         <v>3</v>
       </c>
       <c r="D9" s="88" t="n">
         <f aca="false">IF(Structură!B9, Structură!B9 * Structură!C9, "")</f>
-        <v>180</v>
+        <v>216</v>
       </c>
       <c r="E9" s="101" t="n">
         <v>10.75</v>
       </c>
       <c r="F9" s="101" t="n">
         <f aca="false">IF(Structură!B9, Structură!B9 * Structură!E9, "")</f>
-        <v>645</v>
+        <v>774</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6141,21 +6136,21 @@
         <v>102</v>
       </c>
       <c r="B11" s="86" t="n">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="C11" s="88" t="n">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="D11" s="88" t="n">
         <f aca="false">IF(Structură!B11, Structură!B11 * Structură!C11, "")</f>
-        <v>54</v>
+        <v>180</v>
       </c>
       <c r="E11" s="101" t="n">
-        <v>28.57</v>
+        <v>300</v>
       </c>
       <c r="F11" s="101" t="n">
         <f aca="false">IF(Structură!B11, Structură!B11 * Structură!E11, "")</f>
-        <v>771.39</v>
+        <v>900</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6185,21 +6180,22 @@
         <v>104</v>
       </c>
       <c r="B13" s="86" t="n">
-        <v>8</v>
+        <f aca="false">$I$1</f>
+        <v>12</v>
       </c>
       <c r="C13" s="88" t="n">
         <v>1</v>
       </c>
       <c r="D13" s="88" t="n">
         <f aca="false">IF(Structură!B13, Structură!B13 * Structură!C13, "")</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E13" s="101" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F13" s="101" t="n">
         <f aca="false">IF(Structură!B13, Structură!B13 * Structură!E13, "")</f>
-        <v>200</v>
+        <v>240</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6251,21 +6247,22 @@
         <v>107</v>
       </c>
       <c r="B16" s="86" t="n">
-        <v>0.4</v>
+        <f aca="false">(8 + 4 + 24) * $I$1 + 2 * Circuit!$B$2</f>
+        <v>646</v>
       </c>
       <c r="C16" s="88" t="n">
         <v>0.25</v>
       </c>
       <c r="D16" s="88" t="n">
         <f aca="false">IF(Structură!B16, Structură!B16 * Structură!C16, "")</f>
-        <v>0.1</v>
+        <v>161.5</v>
       </c>
       <c r="E16" s="101" t="n">
         <v>0.06</v>
       </c>
       <c r="F16" s="101" t="n">
         <f aca="false">IF(Structură!B16, Structură!B16 * Structură!E16, "")</f>
-        <v>0.024</v>
+        <v>38.76</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6295,22 +6292,22 @@
         <v>109</v>
       </c>
       <c r="B18" s="86" t="n">
-        <f aca="false">B19+B20+B21+8*B7</f>
-        <v>240</v>
+        <f aca="false">16 * $I$1 + 2 * Circuit!$B$2</f>
+        <v>406</v>
       </c>
       <c r="C18" s="88" t="n">
         <v>0.2</v>
       </c>
       <c r="D18" s="88" t="n">
         <f aca="false">IF(Structură!B18, Structură!B18 * Structură!C18, "")</f>
-        <v>48</v>
-      </c>
-      <c r="E18" s="114" t="n">
+        <v>81.2</v>
+      </c>
+      <c r="E18" s="101" t="n">
         <v>0.03</v>
       </c>
       <c r="F18" s="101" t="n">
         <f aca="false">IF(Structură!B18, Structură!B18 * Structură!E18, "")</f>
-        <v>7.2</v>
+        <v>12.18</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6318,22 +6315,22 @@
         <v>110</v>
       </c>
       <c r="B19" s="86" t="n">
-        <f aca="false">B7 * 4</f>
-        <v>48</v>
+        <f aca="false">8 * $I$1</f>
+        <v>96</v>
       </c>
       <c r="C19" s="88" t="n">
         <v>0.2</v>
       </c>
       <c r="D19" s="88" t="n">
         <f aca="false">IF(Structură!B19, Structură!B19 * Structură!C19, "")</f>
-        <v>9.6</v>
+        <v>19.2</v>
       </c>
       <c r="E19" s="101" t="n">
-        <v>0.03</v>
+        <v>0.0625</v>
       </c>
       <c r="F19" s="101" t="n">
         <f aca="false">IF(Structură!B19, Structură!B19 * Structură!E19, "")</f>
-        <v>1.44</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6341,7 +6338,7 @@
         <v>111</v>
       </c>
       <c r="B20" s="86" t="n">
-        <f aca="false">B7 * 4</f>
+        <f aca="false">4 * $I$1</f>
         <v>48</v>
       </c>
       <c r="C20" s="88" t="n">
@@ -6364,22 +6361,22 @@
         <v>112</v>
       </c>
       <c r="B21" s="86" t="n">
-        <f aca="false">B7 * 4</f>
-        <v>48</v>
+        <f aca="false">8 * $I$1 + 2 * Circuit!$B$2</f>
+        <v>310</v>
       </c>
       <c r="C21" s="88" t="n">
         <v>0.25</v>
       </c>
       <c r="D21" s="88" t="n">
         <f aca="false">IF(Structură!B21, Structură!B21 * Structură!C21, "")</f>
-        <v>12</v>
+        <v>77.5</v>
       </c>
       <c r="E21" s="101" t="n">
         <v>0.125</v>
       </c>
       <c r="F21" s="101" t="n">
         <f aca="false">IF(Structură!B21, Structură!B21 * Structură!E21, "")</f>
-        <v>6</v>
+        <v>38.75</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6387,21 +6384,21 @@
         <v>113</v>
       </c>
       <c r="B22" s="86" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C22" s="88" t="n">
         <v>0.25</v>
       </c>
-      <c r="D22" s="88" t="n">
+      <c r="D22" s="88" t="str">
         <f aca="false">IF(Structură!B22, Structură!B22 * Structură!C22, "")</f>
-        <v>0.5</v>
+        <v/>
       </c>
       <c r="E22" s="101" t="n">
         <v>0.2</v>
       </c>
-      <c r="F22" s="101" t="n">
+      <c r="F22" s="101" t="str">
         <f aca="false">IF(Structură!B22, Structură!B22 * Structură!E22, "")</f>
-        <v>0.4</v>
+        <v/>
       </c>
     </row>
     <row r="23" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6409,21 +6406,21 @@
         <v>114</v>
       </c>
       <c r="B23" s="86" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C23" s="88" t="n">
         <v>0.29</v>
       </c>
-      <c r="D23" s="88" t="n">
+      <c r="D23" s="88" t="str">
         <f aca="false">IF(Structură!B23, Structură!B23 * Structură!C23, "")</f>
-        <v>0.58</v>
+        <v/>
       </c>
       <c r="E23" s="101" t="n">
         <v>0.35</v>
       </c>
-      <c r="F23" s="101" t="n">
+      <c r="F23" s="101" t="str">
         <f aca="false">IF(Structură!B23, Structură!B23 * Structură!E23, "")</f>
-        <v>0.7</v>
+        <v/>
       </c>
     </row>
     <row r="24" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8320,10 +8317,10 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="19.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="19.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="84" width="30.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="86" width="16.81"/>
@@ -8381,11 +8378,11 @@
       </c>
       <c r="E2" s="120" t="n">
         <f aca="true">IF(SUM(INDIRECT(Carcasă!E1)), AVERAGE(INDIRECT(Carcasă!E1)), "")</f>
-        <v>201.25</v>
+        <v>161.25</v>
       </c>
       <c r="F2" s="120" t="n">
         <f aca="true">IF(SUM(INDIRECT(Carcasă!F1)), SUM(INDIRECT(Carcasă!F1)), "")</f>
-        <v>1365</v>
+        <v>1125</v>
       </c>
       <c r="G2" s="103"/>
     </row>
@@ -8411,7 +8408,7 @@
     </row>
     <row r="4" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="84" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="B4" s="86" t="n">
         <v>3</v>
@@ -8424,16 +8421,16 @@
         <v>180</v>
       </c>
       <c r="E4" s="101" t="n">
-        <v>380</v>
+        <v>300</v>
       </c>
       <c r="F4" s="101" t="n">
         <f aca="false">IF(Carcasă!B4, Carcasă!B4 * Carcasă!E4, "")</f>
-        <v>1140</v>
+        <v>900</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="84" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5" s="86" t="n">
         <v>10</v>
@@ -10382,7 +10379,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="19.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="19.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="84" width="55.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="86" width="16.81"/>
@@ -10424,7 +10421,7 @@
     </row>
     <row r="2" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="123" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B2" s="124" t="n">
         <f aca="true">IF(SUM(INDIRECT(Telecomandă!B1)), SUM(INDIRECT(Telecomandă!B1)), "")</f>
@@ -10536,7 +10533,7 @@
     </row>
     <row r="7" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="84" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B7" s="86" t="n">
         <v>1</v>

</xml_diff>